<commit_message>
fixed and made some new directories
</commit_message>
<xml_diff>
--- a/fund_statement_extractor/output/easyocr/final_outputs/flare_extraction_marked.xlsx
+++ b/fund_statement_extractor/output/easyocr/final_outputs/flare_extraction_marked.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinjonany/Desktop/python/data-science/projects/RAG Techniques/FLARE-Implementation/fund_statement_extractor/output/easyocr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinjonany/Desktop/python/data-science/projects/RAG Techniques/FLARE-Implementation/fund_statement_extractor/output/easyocr/final_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E31EFA-FB25-0D4C-A52A-695F8A8B6927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CACBEF-2BE2-4D45-81B2-92D5B5B65C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="500" windowWidth="14280" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1262,7 +1262,7 @@
       <c r="V5" t="s">
         <v>68</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="W5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="X5" t="s">

</xml_diff>